<commit_message>
second project + README
</commit_message>
<xml_diff>
--- a/projects/1_excel-pipeline/data.xlsx
+++ b/projects/1_excel-pipeline/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CGM\Faro\RProjects\4_Cgm\projects\1_excel-pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD89C30B-E5E8-4D51-8E25-6D851EE6C917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B8E2F7-3900-42BD-A7CE-48133525C832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34215" yWindow="0" windowWidth="17385" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,12 +29,12 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Carlos - Vista personalizada" guid="{9DDD3B43-847F-442C-8813-E52402279CDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Vicente CGM - Vista personalizada" guid="{0A9FEBBC-D2A3-457B-A2EA-C6C5DBF86E8A}" mergeInterval="0" personalView="1" xWindow="78" yWindow="22" windowWidth="1250" windowHeight="646" activeSheetId="2"/>
+    <customWorkbookView name="Antonio Sanchez - Vista personalizada" guid="{F5B74D5C-98FD-4D8D-9BF0-BED5A2C78769}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1038" activeSheetId="2"/>
+    <customWorkbookView name="Mariano - Vista personalizada" guid="{84FE4AF5-E5EF-4E71-9E6F-BB14D395BD30}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="JAVIER MIGAL LANAGRAN - Personal View" guid="{AAB38405-2CF3-471C-9510-EF286DC2A9BB}" mergeInterval="0" personalView="1" maximized="1" xWindow="1672" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
     <customWorkbookView name="CGM - Vista personalizada" guid="{E8F90BBB-D2EC-4339-83DB-4A9201C4A218}" mergeInterval="0" personalView="1" windowWidth="1146" windowHeight="1440" activeSheetId="2"/>
-    <customWorkbookView name="JAVIER MIGAL LANAGRAN - Personal View" guid="{AAB38405-2CF3-471C-9510-EF286DC2A9BB}" mergeInterval="0" personalView="1" maximized="1" xWindow="1672" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Mariano - Vista personalizada" guid="{84FE4AF5-E5EF-4E71-9E6F-BB14D395BD30}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Antonio Sanchez - Vista personalizada" guid="{F5B74D5C-98FD-4D8D-9BF0-BED5A2C78769}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1038" activeSheetId="2"/>
-    <customWorkbookView name="Vicente CGM - Vista personalizada" guid="{0A9FEBBC-D2A3-457B-A2EA-C6C5DBF86E8A}" mergeInterval="0" personalView="1" xWindow="78" yWindow="22" windowWidth="1250" windowHeight="646" activeSheetId="2"/>
-    <customWorkbookView name="Carlos - Vista personalizada" guid="{9DDD3B43-847F-442C-8813-E52402279CDB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -677,7 +677,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -722,9 +722,9 @@
       <c r="B3" s="8">
         <v>3.54</v>
       </c>
-      <c r="C3" s="8">
-        <f>B3</f>
-        <v>3.54</v>
+      <c r="C3" s="8" t="e">
+        <f>+B4*3</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D3" s="7">
         <v>45595</v>
@@ -752,6 +752,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="feb1dc68-0493-488a-806e-c97c65915c9f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="fef048ad-ab74-4dc9-aeb1-5a2368d3adfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CBC66022B88D67498CE02E70E50AB7CC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d9a8e4ed6e24e522584ecbfcc09c6095">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="feb1dc68-0493-488a-806e-c97c65915c9f" xmlns:ns3="fef048ad-ab74-4dc9-aeb1-5a2368d3adfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fc8b908f8d62b004d26e10d1481b0e8" ns2:_="" ns3:_="">
     <xsd:import namespace="feb1dc68-0493-488a-806e-c97c65915c9f"/>
@@ -940,17 +951,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="feb1dc68-0493-488a-806e-c97c65915c9f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="fef048ad-ab74-4dc9-aeb1-5a2368d3adfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -961,6 +961,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E11DEA0-B82F-4826-BE1E-527DEB582657}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="feb1dc68-0493-488a-806e-c97c65915c9f"/>
+    <ds:schemaRef ds:uri="fef048ad-ab74-4dc9-aeb1-5a2368d3adfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B169D707-5693-48D9-9D37-1907E9B95328}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -979,17 +990,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E11DEA0-B82F-4826-BE1E-527DEB582657}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="feb1dc68-0493-488a-806e-c97c65915c9f"/>
-    <ds:schemaRef ds:uri="fef048ad-ab74-4dc9-aeb1-5a2368d3adfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E51DD3C7-1DEA-426F-A948-F904BD18B778}">
   <ds:schemaRefs>

</xml_diff>